<commit_message>
added ADXL372BCCZ-RL. Removed non-used signals (int1/int2) from IMUS.
</commit_message>
<xml_diff>
--- a/RP2040_GPIO_config.xlsx
+++ b/RP2040_GPIO_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Engineering work\blackmagic\L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E906CF88-A531-4C97-A32B-0CF9D8900459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C969D4C1-312F-403F-AB67-4DA3D3174AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57600" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{B2E1D852-938E-4C87-BD26-E74864A2E1E1}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="100">
   <si>
     <t>GPIO</t>
   </si>
@@ -181,12 +181,6 @@
     <t>I2C1 SCL</t>
   </si>
   <si>
-    <t>CLOCK GPIN0</t>
-  </si>
-  <si>
-    <t>CLOCK GPOUT0</t>
-  </si>
-  <si>
     <t>CLOCK GPIN1</t>
   </si>
   <si>
@@ -316,12 +310,6 @@
     <t>IMU2 - CSn</t>
   </si>
   <si>
-    <t>IMU1 - INT1</t>
-  </si>
-  <si>
-    <t>IMU2 - INT1</t>
-  </si>
-  <si>
     <t>IMU - MISO</t>
   </si>
   <si>
@@ -346,18 +334,9 @@
     <t>BARO - MOSI</t>
   </si>
   <si>
-    <t>XCO</t>
-  </si>
-  <si>
-    <t>TCO</t>
-  </si>
-  <si>
     <t>BARO2 - CSn</t>
   </si>
   <si>
-    <t>GPS - UART SEL</t>
-  </si>
-  <si>
     <t>GPS - SDA</t>
   </si>
   <si>
@@ -407,6 +386,12 @@
   </si>
   <si>
     <t>PYRO 2 Sense</t>
+  </si>
+  <si>
+    <t>High G IMU SDA</t>
+  </si>
+  <si>
+    <t>High G IMU SCL</t>
   </si>
 </sst>
 </file>
@@ -795,7 +780,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -831,7 +816,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -843,10 +828,10 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -863,25 +848,25 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
         <v>52</v>
       </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" t="s">
-        <v>54</v>
-      </c>
       <c r="L2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="M2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -898,25 +883,25 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
       <c r="L3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="M3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -933,25 +918,25 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="M4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -968,25 +953,25 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
-      </c>
       <c r="L5" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="M5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1003,25 +988,25 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
         <v>53</v>
       </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
       <c r="L6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1038,25 +1023,25 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="M7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1073,25 +1058,25 @@
         <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="s">
-        <v>54</v>
-      </c>
       <c r="L8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1108,25 +1093,25 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
         <v>53</v>
       </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
       <c r="L9" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="M9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1143,25 +1128,25 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="M10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1178,25 +1163,25 @@
         <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" t="s">
         <v>52</v>
       </c>
-      <c r="I11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
       <c r="L11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="M11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1209,29 +1194,29 @@
       <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
         <v>53</v>
       </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
       <c r="L12" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1244,29 +1229,29 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="M13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1283,25 +1268,25 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" t="s">
-        <v>54</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="M14" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1318,25 +1303,22 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
         <v>53</v>
       </c>
-      <c r="K15" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" t="s">
-        <v>75</v>
-      </c>
       <c r="M15" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1353,25 +1335,25 @@
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="M16" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1388,25 +1370,25 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" t="s">
-        <v>54</v>
-      </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M17" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1423,25 +1405,25 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" t="s">
         <v>53</v>
       </c>
-      <c r="K18" t="s">
-        <v>55</v>
-      </c>
       <c r="L18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="M18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1458,25 +1440,25 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M19" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1493,25 +1475,25 @@
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" t="s">
         <v>52</v>
       </c>
-      <c r="I20" t="s">
-        <v>53</v>
-      </c>
-      <c r="K20" t="s">
-        <v>54</v>
-      </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M20" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1528,25 +1510,25 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I21" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" t="s">
         <v>53</v>
       </c>
-      <c r="K21" t="s">
-        <v>55</v>
-      </c>
       <c r="L21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1563,28 +1545,23 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="2"/>
       <c r="K22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="M22" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1601,28 +1578,23 @@
         <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" t="s">
         <v>52</v>
       </c>
-      <c r="I23" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" t="s">
-        <v>54</v>
-      </c>
-      <c r="L23" t="s">
-        <v>85</v>
-      </c>
       <c r="M23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1639,28 +1611,28 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K24" t="s">
-        <v>55</v>
-      </c>
       <c r="L24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M24" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1677,28 +1649,28 @@
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="M25" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1715,28 +1687,28 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" t="s">
         <v>52</v>
       </c>
-      <c r="I26" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" t="s">
-        <v>33</v>
-      </c>
-      <c r="K26" t="s">
-        <v>54</v>
-      </c>
       <c r="L26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M26" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1753,28 +1725,28 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
         <v>53</v>
       </c>
-      <c r="J27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" t="s">
-        <v>55</v>
-      </c>
       <c r="L27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M27" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1791,25 +1763,25 @@
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M28" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1826,25 +1798,25 @@
         <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" t="s">
         <v>52</v>
       </c>
-      <c r="I29" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" t="s">
-        <v>54</v>
-      </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M29" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1861,25 +1833,25 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30" t="s">
         <v>53</v>
       </c>
-      <c r="K30" t="s">
-        <v>55</v>
-      </c>
       <c r="L30" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="M30" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1896,96 +1868,96 @@
         <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L31" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="M31" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>